<commit_message>
Added support for Nanosurf AFM and STM .nid files
</commit_message>
<xml_diff>
--- a/tests/test_files/1_lab_journal.xlsx
+++ b/tests/test_files/1_lab_journal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga26jul\github\proespm-py3\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641D0330-D20C-4E3B-A173-4967513D1DE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8943B6-CC28-4FA0-A02C-F9B2EFF04302}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="76">
   <si>
     <t>day</t>
   </si>
@@ -238,16 +238,28 @@
   </si>
   <si>
     <t>LEED .png file</t>
+  </si>
+  <si>
+    <t>stm-nanosurf-nid</t>
+  </si>
+  <si>
+    <t>afm-nanosurf-nid</t>
+  </si>
+  <si>
+    <t>afm</t>
+  </si>
+  <si>
+    <t>Nanosurf AFM .nid file</t>
+  </si>
+  <si>
+    <t>Nanosurf STM .nid file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -260,6 +272,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -282,11 +300,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -294,6 +312,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,7 +632,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,10 +1110,32 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="2"/>
+      <c r="A26" s="1">
+        <v>45098</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
+      <c r="A27" s="1">
+        <v>45098</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
@@ -1233,6 +1275,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deleted unnecessary test files
</commit_message>
<xml_diff>
--- a/tests/test_files/1_lab_journal.xlsx
+++ b/tests/test_files/1_lab_journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga26jul\github\proespm-py3\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB1663C-8862-49A3-BCFA-1BB081A43307}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068C52C5-E6F2-4F88-9985-3ADB4D646DDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="93">
   <si>
     <t>day</t>
   </si>
@@ -108,18 +108,12 @@
     <t>15.05.2021</t>
   </si>
   <si>
-    <t>png-a</t>
-  </si>
-  <si>
     <t>image</t>
   </si>
   <si>
     <t>.png file</t>
   </si>
   <si>
-    <t>png-b</t>
-  </si>
-  <si>
     <t>02.07.2021</t>
   </si>
   <si>
@@ -307,6 +301,9 @@
   </si>
   <si>
     <t>.jpeg file</t>
+  </si>
+  <si>
+    <t>png_test</t>
   </si>
 </sst>
 </file>
@@ -687,11 +684,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMM73"/>
+  <dimension ref="A1:AMM72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -941,230 +938,230 @@
         <v>26</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="2" t="s">
+    </row>
+    <row r="13" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="E14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="E15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="E16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>11</v>
+        <v>43</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>42</v>
+        <v>13</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>49</v>
+        <v>11</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>55</v>
+        <v>13</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>11</v>
+        <v>56</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="A25" s="1">
+        <v>45098</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="C25" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" s="11" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1176,35 +1173,35 @@
         <v>71</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>45098</v>
-      </c>
-      <c r="B27" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="11" t="s">
+    </row>
+    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="B27" s="3" t="s">
         <v>75</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>79</v>
@@ -1212,41 +1209,41 @@
     </row>
     <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I30" s="8" t="s">
         <v>85</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>88</v>
@@ -1254,66 +1251,55 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I32" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="8"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="8"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" s="8"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="8"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="8"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="8"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" s="8"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="8"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="8"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="8"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" s="8"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" s="8"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">
@@ -1387,9 +1373,6 @@
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" s="8"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B73" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Added test files for LabView written Electrochemistry
</commit_message>
<xml_diff>
--- a/tests/test_files/1_lab_journal.xlsx
+++ b/tests/test_files/1_lab_journal.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga26jul\github\proespm-py3\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068C52C5-E6F2-4F88-9985-3ADB4D646DDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3000B2-B657-4E80-AE54-4E35820840B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterate="1" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="105">
   <si>
     <t>day</t>
   </si>
@@ -304,6 +304,42 @@
   </si>
   <si>
     <t>png_test</t>
+  </si>
+  <si>
+    <t>20.07.2023</t>
+  </si>
+  <si>
+    <t>CV_50mvs_001</t>
+  </si>
+  <si>
+    <t>cv_lv</t>
+  </si>
+  <si>
+    <t>Cyclic Voltammetry ECSTM (LabVIEW)</t>
+  </si>
+  <si>
+    <t>27.02.2018</t>
+  </si>
+  <si>
+    <t>CA_Pulse-Time-4_01</t>
+  </si>
+  <si>
+    <t>ca_lv</t>
+  </si>
+  <si>
+    <t>Chronoamperometry ECSTM (LabVIEW)</t>
+  </si>
+  <si>
+    <t>FFT_test</t>
+  </si>
+  <si>
+    <t>fft_lv</t>
+  </si>
+  <si>
+    <t>25.05.2023</t>
+  </si>
+  <si>
+    <t>FFT ECSTM (LabVIEW) - try to show only up to 2 kHz to visualize most relevant noise</t>
   </si>
 </sst>
 </file>
@@ -688,7 +724,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
+      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1251,55 +1287,97 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="I33" s="8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B36" s="8"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B37" s="8"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B38" s="8"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B39" s="8"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B40" s="8"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B41" s="8"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B42" s="8"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B44" s="8"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B45" s="8"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B46" s="8"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B47" s="8"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B48" s="8"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>